<commit_message>
add Jerry to do
</commit_message>
<xml_diff>
--- a/002_FaaS_Chengdu_current_issue.xlsx
+++ b/002_FaaS_Chengdu_current_issue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="My Task" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Incident 1570738798</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Jerry comment</t>
   </si>
   <si>
-    <t>I replied to Ishan that for measured roundtrip, only 3 roundtrips could be regarded as application sequential roundtrips.</t>
-  </si>
-  <si>
     <t>STEP 3. Select a task</t>
   </si>
   <si>
@@ -70,16 +67,56 @@
   </si>
   <si>
     <t>STEP7 Click on EDIT</t>
+  </si>
+  <si>
+    <t>Hyperlink</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>I replied to Ishan that for measured roundtrip, only 3 roundtrips could be regarded as application sequential roundtrips.
+Angela has doubt about request #5. 
+See detail in hyperlink.</t>
+  </si>
+  <si>
+    <t>TODO(Jerry):</t>
+  </si>
+  <si>
+    <t>1. in STEP 1, currently the batch request( technical detail, priority and user status) is sequentially before task list retrieval. Check whether parallem processing of</t>
+  </si>
+  <si>
+    <t>both is possible.</t>
+  </si>
+  <si>
+    <t>1. check whether it is the common procedure to check the edit authorization in a separate roundtrip in the beginning</t>
+  </si>
+  <si>
+    <t>2. check Angela's comment on 3 measured roundtrip.</t>
+  </si>
+  <si>
+    <t>1. in STEP 1. check whether it is possible to delay the retrieval of user status and priority until an opportunity is edited.</t>
+  </si>
+  <si>
+    <t>2. check why there are 8 roundtrips measured when opp is opened.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,17 +145,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,18 +474,22 @@
     <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="22.44140625" customWidth="1"/>
     <col min="5" max="5" width="24.77734375" customWidth="1"/>
-    <col min="6" max="6" width="53.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="44.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -459,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -476,12 +520,15 @@
         <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>1.851</v>
@@ -490,18 +537,34 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +578,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -523,7 +586,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -534,7 +597,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>8.2520000000000007</v>
@@ -551,7 +614,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>4.1710000000000003</v>
@@ -562,7 +625,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
         <v>2.0760000000000001</v>
@@ -573,13 +636,26 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>2.2000000000000002</v>
       </c>
       <c r="C9">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -589,10 +665,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,7 +682,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -614,7 +690,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -625,7 +701,7 @@
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>2.08</v>
@@ -636,7 +712,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>2.2999999999999998</v>
@@ -649,6 +725,19 @@
       </c>
       <c r="E5">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new example under CBA pressure
</commit_message>
<xml_diff>
--- a/002_FaaS_Chengdu_current_issue.xlsx
+++ b/002_FaaS_Chengdu_current_issue.xlsx
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,7 +564,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>